<commit_message>
Commands 0 to 7 implemented
</commit_message>
<xml_diff>
--- a/adress mapping.xlsx
+++ b/adress mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafaelpetter\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafaelpetter\Documents\GitHub\Electrocelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62DDEFC-38C6-4066-B3BD-9A3446C05C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B076E2A0-30A6-46F8-91C9-1979ABD9CA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="2685" windowWidth="15330" windowHeight="10890" activeTab="1" xr2:uid="{3A93FA6F-FB22-4E72-B6B6-97C9E5C36F6A}"/>
+    <workbookView xWindow="-28755" yWindow="405" windowWidth="57390" windowHeight="14985" activeTab="1" xr2:uid="{3A93FA6F-FB22-4E72-B6B6-97C9E5C36F6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Table" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="114">
   <si>
     <t>decelarationOpen</t>
   </si>
@@ -374,13 +374,16 @@
   </si>
   <si>
     <t>command ID</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,8 +411,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +492,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -924,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1020,6 +1042,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1035,7 +1077,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1045,37 +1092,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCCC"/>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1405,10 +1448,10 @@
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="37"/>
+      <c r="G2" s="45"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1438,7 +1481,7 @@
       <c r="C4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="43">
         <v>10</v>
       </c>
       <c r="E4" s="10">
@@ -1458,7 +1501,7 @@
       <c r="C5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="12">
         <v>0</v>
       </c>
@@ -1476,7 +1519,7 @@
       <c r="C6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="41">
         <v>11</v>
       </c>
       <c r="E6" s="12">
@@ -1496,7 +1539,7 @@
       <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="12">
         <v>0</v>
       </c>
@@ -1534,7 +1577,7 @@
       <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="41">
         <v>13</v>
       </c>
       <c r="E9" s="12">
@@ -1554,7 +1597,7 @@
       <c r="C10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="12">
         <v>0</v>
       </c>
@@ -1572,7 +1615,7 @@
       <c r="C11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="41">
         <v>14</v>
       </c>
       <c r="E11" s="12">
@@ -1592,7 +1635,7 @@
       <c r="C12" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="12">
         <v>0</v>
       </c>
@@ -1610,7 +1653,7 @@
       <c r="C13" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="41">
         <v>15</v>
       </c>
       <c r="E13" s="12">
@@ -1630,7 +1673,7 @@
       <c r="C14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="12">
         <v>0</v>
       </c>
@@ -1788,7 +1831,7 @@
       <c r="C22" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="41" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="12">
@@ -1808,7 +1851,7 @@
       <c r="C23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="34"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="12">
         <v>0</v>
       </c>
@@ -1986,7 +2029,7 @@
       <c r="C32" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="35">
+      <c r="D32" s="43">
         <v>26</v>
       </c>
       <c r="E32" s="13">
@@ -2006,7 +2049,7 @@
       <c r="C33" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="34"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="12">
         <v>0</v>
       </c>
@@ -2197,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9ED7B76-3A63-4D9B-8370-285AECF4CE1B}">
   <dimension ref="A2:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,435 +2254,466 @@
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="33"/>
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="33"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="43" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="33"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="44" t="s">
+      <c r="A5" s="33"/>
+      <c r="B5" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
+      <c r="J5" s="54">
+        <v>1</v>
+      </c>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="33"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="44" t="s">
+      <c r="A6" s="33"/>
+      <c r="B6" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="38"/>
-      <c r="Z6" s="38"/>
+      <c r="J6" s="54">
+        <v>1</v>
+      </c>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="33"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="44" t="s">
+      <c r="A7" s="33"/>
+      <c r="B7" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="G7" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="38"/>
-      <c r="W7" s="38"/>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38"/>
-      <c r="Z7" s="38"/>
+      <c r="J7" s="54">
+        <v>1</v>
+      </c>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="44" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="48" t="s">
+      <c r="H8" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="38" t="s">
         <v>76</v>
       </c>
+      <c r="J8" s="55">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="44" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="47" t="s">
+      <c r="E9" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="48" t="s">
+      <c r="H9" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="38" t="s">
         <v>76</v>
       </c>
+      <c r="J9" s="55">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="44" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="47" t="s">
+      <c r="G10" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="48" t="s">
+      <c r="H10" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="I10" s="47" t="s">
+      <c r="I10" s="38" t="s">
         <v>76</v>
       </c>
+      <c r="J10" s="55">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="44" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="I11" s="47" t="s">
+      <c r="I11" s="38" t="s">
         <v>76</v>
       </c>
+      <c r="J11" s="55">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="44" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="47" t="s">
+      <c r="F12" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="47" t="s">
+      <c r="G12" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="H12" s="48" t="s">
+      <c r="H12" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="I12" s="47" t="s">
+      <c r="I12" s="38" t="s">
         <v>76</v>
       </c>
+      <c r="J12" s="55">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="H13" s="50" t="s">
+      <c r="H13" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="I13" s="47" t="s">
+      <c r="I13" s="38" t="s">
         <v>76</v>
       </c>
+      <c r="J13" s="55">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="47" t="s">
+      <c r="F14" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="47" t="s">
+      <c r="G14" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="H14" s="47" t="s">
+      <c r="H14" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="38" t="s">
         <v>76</v>
       </c>
+      <c r="J14" s="55">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B2:I2"/>
+  <mergeCells count="6">
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added command read serial
</commit_message>
<xml_diff>
--- a/adress mapping.xlsx
+++ b/adress mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafaelpetter\Documents\GitHub\Electrocelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91F46A3-AD6D-45AF-A924-B612F13E68A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813A3FFD-AD06-4514-AC3C-2BCF4784D495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3A93FA6F-FB22-4E72-B6B6-97C9E5C36F6A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="116">
   <si>
     <t>decelarationOpen</t>
   </si>
@@ -376,7 +376,13 @@
     <t>done</t>
   </si>
   <si>
-    <t>command ID (1st half then 2nd half)</t>
+    <t>read serial</t>
+  </si>
+  <si>
+    <t>read the serial of a saved command</t>
+  </si>
+  <si>
+    <t>serial (1st half then 2nd half)</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -942,11 +948,131 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1043,31 +1169,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1083,28 +1184,64 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1448,10 +1585,10 @@
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="47"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1481,7 +1618,7 @@
       <c r="C4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="36">
         <v>10</v>
       </c>
       <c r="E4" s="10">
@@ -1501,7 +1638,7 @@
       <c r="C5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="12">
         <v>0</v>
       </c>
@@ -1519,7 +1656,7 @@
       <c r="C6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="34">
         <v>11</v>
       </c>
       <c r="E6" s="12">
@@ -1539,7 +1676,7 @@
       <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="44"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="12">
         <v>0</v>
       </c>
@@ -1577,7 +1714,7 @@
       <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="34">
         <v>13</v>
       </c>
       <c r="E9" s="12">
@@ -1597,7 +1734,7 @@
       <c r="C10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="12">
         <v>0</v>
       </c>
@@ -1615,7 +1752,7 @@
       <c r="C11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="34">
         <v>14</v>
       </c>
       <c r="E11" s="12">
@@ -1635,7 +1772,7 @@
       <c r="C12" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="44"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="12">
         <v>0</v>
       </c>
@@ -1653,7 +1790,7 @@
       <c r="C13" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="34">
         <v>15</v>
       </c>
       <c r="E13" s="12">
@@ -1673,7 +1810,7 @@
       <c r="C14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="44"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="12">
         <v>0</v>
       </c>
@@ -1831,7 +1968,7 @@
       <c r="C22" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="34" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="12">
@@ -1851,7 +1988,7 @@
       <c r="C23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="44"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="12">
         <v>0</v>
       </c>
@@ -2029,7 +2166,7 @@
       <c r="C32" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="45">
+      <c r="D32" s="36">
         <v>26</v>
       </c>
       <c r="E32" s="13">
@@ -2049,7 +2186,7 @@
       <c r="C33" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="44"/>
+      <c r="D33" s="35"/>
       <c r="E33" s="12">
         <v>0</v>
       </c>
@@ -2238,10 +2375,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9ED7B76-3A63-4D9B-8370-285AECF4CE1B}">
-  <dimension ref="A2:Z14"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,18 +2394,19 @@
     <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
       <c r="K2" s="33"/>
       <c r="L2" s="33"/>
       <c r="M2" s="33"/>
@@ -2287,23 +2425,23 @@
       <c r="Z2" s="33"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="53" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="51" t="s">
         <v>112</v>
       </c>
       <c r="K3" s="33"/>
@@ -2324,25 +2462,25 @@
       <c r="Z3" s="33"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="34" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="53"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
@@ -2362,31 +2500,31 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="53">
         <v>1</v>
       </c>
       <c r="K5" s="33"/>
@@ -2408,31 +2546,31 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="41">
+      <c r="J6" s="53">
         <v>1</v>
       </c>
       <c r="K6" s="33"/>
@@ -2454,31 +2592,31 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="33"/>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="53">
         <v>1</v>
       </c>
       <c r="K7" s="33"/>
@@ -2500,209 +2638,238 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="53">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="53">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="33"/>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="I10" s="38" t="s">
+      <c r="I10" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="53">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="54" t="s">
+      <c r="H11" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I11" s="38" t="s">
+      <c r="I11" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="53">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="33"/>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="55" t="s">
+      <c r="G12" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="H12" s="54" t="s">
+      <c r="H12" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="42">
+      <c r="J12" s="53">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="H13" s="40" t="s">
+      <c r="H13" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="I13" s="38" t="s">
+      <c r="D15" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="J13" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="H14" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="I14" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14" s="42">
+      <c r="J15" s="58">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added state machine states to read command
</commit_message>
<xml_diff>
--- a/adress mapping.xlsx
+++ b/adress mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafaelpetter\Documents\GitHub\Electrocelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813A3FFD-AD06-4514-AC3C-2BCF4784D495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333F8BC1-FBC8-4617-BC08-5478EC8B54E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3A93FA6F-FB22-4E72-B6B6-97C9E5C36F6A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A93FA6F-FB22-4E72-B6B6-97C9E5C36F6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Table" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="128">
   <si>
     <t>decelarationOpen</t>
   </si>
@@ -383,13 +383,49 @@
   </si>
   <si>
     <t>serial (1st half then 2nd half)</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>0x0F</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Walk</t>
+  </si>
+  <si>
+    <t>s_ControlGate</t>
+  </si>
+  <si>
+    <t>s_ControlLearning</t>
+  </si>
+  <si>
+    <t>s_Main</t>
+  </si>
+  <si>
+    <t>s_MenuConfiguration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,6 +456,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -511,7 +554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -964,13 +1007,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -979,93 +1020,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right/>
+      <top style="hair">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1169,6 +1131,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1184,64 +1167,41 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1564,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6891E5-FE77-48FB-B78B-775FB6629AE6}">
-  <dimension ref="B1:H41"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,10 +1545,10 @@
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="38"/>
+      <c r="G2" s="45"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1618,7 +1578,7 @@
       <c r="C4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="43">
         <v>10</v>
       </c>
       <c r="E4" s="10">
@@ -1638,7 +1598,7 @@
       <c r="C5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="12">
         <v>0</v>
       </c>
@@ -1656,7 +1616,7 @@
       <c r="C6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="41">
         <v>11</v>
       </c>
       <c r="E6" s="12">
@@ -1676,7 +1636,7 @@
       <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="12">
         <v>0</v>
       </c>
@@ -1714,7 +1674,7 @@
       <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="41">
         <v>13</v>
       </c>
       <c r="E9" s="12">
@@ -1734,7 +1694,7 @@
       <c r="C10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="12">
         <v>0</v>
       </c>
@@ -1752,7 +1712,7 @@
       <c r="C11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="41">
         <v>14</v>
       </c>
       <c r="E11" s="12">
@@ -1772,7 +1732,7 @@
       <c r="C12" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="35"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="12">
         <v>0</v>
       </c>
@@ -1790,7 +1750,7 @@
       <c r="C13" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="41">
         <v>15</v>
       </c>
       <c r="E13" s="12">
@@ -1810,7 +1770,7 @@
       <c r="C14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="35"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="12">
         <v>0</v>
       </c>
@@ -1968,7 +1928,7 @@
       <c r="C22" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="41" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="12">
@@ -1988,7 +1948,7 @@
       <c r="C23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="35"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="12">
         <v>0</v>
       </c>
@@ -2166,7 +2126,7 @@
       <c r="C32" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D32" s="43">
         <v>26</v>
       </c>
       <c r="E32" s="13">
@@ -2179,14 +2139,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="29">
         <v>1</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="35"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="12">
         <v>0</v>
       </c>
@@ -2197,7 +2157,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="29">
         <v>8</v>
       </c>
@@ -2217,7 +2177,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="29">
         <v>1</v>
       </c>
@@ -2237,7 +2197,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="29">
         <v>8</v>
       </c>
@@ -2257,7 +2217,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="31">
         <v>8</v>
       </c>
@@ -2277,7 +2237,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="29">
         <v>4</v>
       </c>
@@ -2297,7 +2257,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="29">
         <v>4</v>
       </c>
@@ -2317,7 +2277,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="29">
         <v>8</v>
       </c>
@@ -2337,7 +2297,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="30">
         <v>8</v>
       </c>
@@ -2356,6 +2316,69 @@
       <c r="G41" s="18" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="29">
+        <v>1</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="16">
+        <v>34</v>
+      </c>
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="29">
+        <v>1</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" s="16">
+        <v>34</v>
+      </c>
+      <c r="E44" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="29">
+        <v>1</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" s="16">
+        <v>35</v>
+      </c>
+      <c r="E45" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="29">
+        <v>1</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="D46" s="54">
+        <v>35</v>
+      </c>
+      <c r="E46" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="55"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2375,39 +2398,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9ED7B76-3A63-4D9B-8370-285AECF4CE1B}">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="B1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+    </row>
+    <row r="2" spans="2:27" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="33"/>
+      <c r="C2" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="33"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="33"/>
       <c r="M2" s="33"/>
       <c r="N2" s="33"/>
@@ -2423,28 +2459,29 @@
       <c r="X2" s="33"/>
       <c r="Y2" s="33"/>
       <c r="Z2" s="33"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="50" t="s">
+      <c r="AA2" s="33"/>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B3" s="33"/>
+      <c r="C3" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="D3" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="E3" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="F3" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="51" t="s">
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="K3" s="33"/>
       <c r="L3" s="33"/>
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
@@ -2460,28 +2497,29 @@
       <c r="X3" s="33"/>
       <c r="Y3" s="33"/>
       <c r="Z3" s="33"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="50"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42" t="s">
+      <c r="AA3" s="33"/>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B4" s="33"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="G4" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="H4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="I4" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="J4" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="51"/>
-      <c r="K4" s="33"/>
+      <c r="K4" s="53"/>
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
       <c r="N4" s="33"/>
@@ -2497,37 +2535,37 @@
       <c r="X4" s="33"/>
       <c r="Y4" s="33"/>
       <c r="Z4" s="33"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="52" t="s">
+      <c r="AA4" s="33"/>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B5" s="33"/>
+      <c r="C5" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="D5" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="E5" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="F5" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="G5" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="H5" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="I5" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="J5" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="53">
-        <v>1</v>
-      </c>
-      <c r="K5" s="33"/>
+      <c r="K5" s="40">
+        <v>1</v>
+      </c>
       <c r="L5" s="33"/>
       <c r="M5" s="33"/>
       <c r="N5" s="33"/>
@@ -2543,37 +2581,37 @@
       <c r="X5" s="33"/>
       <c r="Y5" s="33"/>
       <c r="Z5" s="33"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="52" t="s">
+      <c r="AA5" s="33"/>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B6" s="33"/>
+      <c r="C6" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="D6" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="E6" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="F6" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="45" t="s">
+      <c r="G6" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="H6" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="H6" s="45" t="s">
+      <c r="I6" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="45" t="s">
+      <c r="J6" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="53">
-        <v>1</v>
-      </c>
-      <c r="K6" s="33"/>
+      <c r="K6" s="40">
+        <v>1</v>
+      </c>
       <c r="L6" s="33"/>
       <c r="M6" s="33"/>
       <c r="N6" s="33"/>
@@ -2589,37 +2627,37 @@
       <c r="X6" s="33"/>
       <c r="Y6" s="33"/>
       <c r="Z6" s="33"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="52" t="s">
+      <c r="AA6" s="33"/>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B7" s="33"/>
+      <c r="C7" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="D7" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="E7" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="F7" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="G7" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="H7" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="I7" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="45" t="s">
+      <c r="J7" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="53">
-        <v>1</v>
-      </c>
-      <c r="K7" s="33"/>
+      <c r="K7" s="40">
+        <v>1</v>
+      </c>
       <c r="L7" s="33"/>
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
@@ -2635,252 +2673,526 @@
       <c r="X7" s="33"/>
       <c r="Y7" s="33"/>
       <c r="Z7" s="33"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="52" t="s">
+      <c r="AA7" s="33"/>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B8" s="33"/>
+      <c r="C8" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="D8" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="E8" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="F8" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="G8" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="H8" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="I8" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="J8" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J8" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="52" t="s">
+      <c r="K8" s="40">
+        <v>1</v>
+      </c>
+      <c r="L8" s="33"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B9" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="D9" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="E9" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="F9" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="G9" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="H9" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="45" t="s">
+      <c r="I9" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="45" t="s">
+      <c r="J9" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J9" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="52" t="s">
+      <c r="K9" s="40">
+        <v>1</v>
+      </c>
+      <c r="L9" s="33"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B10" s="46"/>
+      <c r="C10" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="D10" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="E10" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="F10" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="G10" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="45" t="s">
+      <c r="H10" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="I10" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="I10" s="45" t="s">
+      <c r="J10" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="52" t="s">
+      <c r="K10" s="40">
+        <v>1</v>
+      </c>
+      <c r="L10" s="33"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B11" s="46"/>
+      <c r="C11" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="D11" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="E11" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="F11" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="G11" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="46" t="s">
+      <c r="H11" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="I11" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="I11" s="45" t="s">
+      <c r="J11" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="52" t="s">
+      <c r="K11" s="40">
+        <v>1</v>
+      </c>
+      <c r="L11" s="33"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B12" s="46"/>
+      <c r="C12" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="D12" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="E12" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="F12" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="G12" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="H12" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="H12" s="46" t="s">
+      <c r="I12" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="I12" s="45" t="s">
+      <c r="J12" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B13" s="52" t="s">
+      <c r="K12" s="40">
+        <v>1</v>
+      </c>
+      <c r="L12" s="33"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B13" s="46"/>
+      <c r="C13" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="D13" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="E13" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="F13" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="G13" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="G13" s="45" t="s">
+      <c r="H13" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H13" s="45" t="s">
+      <c r="I13" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="I13" s="45" t="s">
+      <c r="J13" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J13" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="52" t="s">
+      <c r="K13" s="40">
+        <v>1</v>
+      </c>
+      <c r="L13" s="33"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B14" s="46"/>
+      <c r="C14" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="D14" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="E14" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="F14" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="G14" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="H14" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H14" s="45" t="s">
+      <c r="I14" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="I14" s="45" t="s">
+      <c r="J14" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="54" t="s">
+      <c r="K14" s="40">
+        <v>1</v>
+      </c>
+      <c r="L14" s="33"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B15" s="46"/>
+      <c r="C15" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="D15" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="56" t="s">
+      <c r="E15" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="F15" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="57" t="s">
+      <c r="G15" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="57" t="s">
+      <c r="H15" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H15" s="57" t="s">
+      <c r="I15" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="I15" s="57" t="s">
+      <c r="J15" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J15" s="58">
-        <v>1</v>
-      </c>
+      <c r="K15" s="40">
+        <v>1</v>
+      </c>
+      <c r="L15" s="33"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B16" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K16" s="40">
+        <v>0</v>
+      </c>
+      <c r="L16" s="33"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
+      <c r="C17" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="40">
+        <v>0</v>
+      </c>
+      <c r="L17" s="33"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="47"/>
+      <c r="C18" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K18" s="40">
+        <v>0</v>
+      </c>
+      <c r="L18" s="33"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="47"/>
+      <c r="C19" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="J19" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K19" s="40">
+        <v>0</v>
+      </c>
+      <c r="L19" s="33"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="47"/>
+      <c r="C20" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="J20" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" s="40">
+        <v>0</v>
+      </c>
+      <c r="L20" s="33"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="47"/>
+      <c r="C21" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I21" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="J21" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K21" s="40">
+        <v>0</v>
+      </c>
+      <c r="L21" s="33"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="47"/>
+      <c r="C22" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="40">
+        <v>0</v>
+      </c>
+      <c r="L22" s="33"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="B3:B4"/>
+  <mergeCells count="8">
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="F3:J3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mid adding new variables to read
</commit_message>
<xml_diff>
--- a/adress mapping.xlsx
+++ b/adress mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafaelpetter\Documents\GitHub\Electrocelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D886D88-17A7-4936-9CFC-3B6857AB17E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999603CA-2961-4622-93E4-8B206C7B7A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A93FA6F-FB22-4E72-B6B6-97C9E5C36F6A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="138">
   <si>
     <t>decelarationOpen</t>
   </si>
@@ -403,180 +403,21 @@
     <t>Walk</t>
   </si>
   <si>
-    <t>s_ControlGate</t>
-  </si>
-  <si>
-    <t>s_ControlLearning</t>
-  </si>
-  <si>
-    <t>s_Main</t>
-  </si>
-  <si>
-    <t>s_MenuConfiguration</t>
-  </si>
-  <si>
-    <t>Rfcount</t>
-  </si>
-  <si>
-    <t>RFstate</t>
-  </si>
-  <si>
-    <t>Bptr</t>
-  </si>
-  <si>
-    <t>BitCount</t>
-  </si>
-  <si>
     <t>RFFull</t>
   </si>
   <si>
-    <t>RFFull_12BIT</t>
-  </si>
-  <si>
-    <t>RFBit</t>
-  </si>
-  <si>
-    <t>FimdeCursoOpenAUX</t>
-  </si>
-  <si>
-    <t>FimdeCursoOpenOLD</t>
-  </si>
-  <si>
-    <t>FimdeCursoOpenTimer</t>
-  </si>
-  <si>
-    <t>FimdeCursoCloseAUX</t>
-  </si>
-  <si>
-    <t>FimdeCursoCloseOLD</t>
-  </si>
-  <si>
-    <t>FimdeCursoCloseTimer</t>
-  </si>
-  <si>
-    <t>PhotoCellAUX</t>
-  </si>
-  <si>
-    <t>PhotoCellOLD</t>
-  </si>
-  <si>
-    <t>PhotoCellTimer</t>
-  </si>
-  <si>
-    <t>SecurityBarAUX</t>
-  </si>
-  <si>
-    <t>SecurityBarOLD</t>
-  </si>
-  <si>
-    <t>SecurityBarTimer</t>
-  </si>
-  <si>
-    <t>SecurityBarSTATE</t>
-  </si>
-  <si>
-    <t>SecurityBar8K2AUX</t>
-  </si>
-  <si>
-    <t>SecurityBar8K2OLD</t>
-  </si>
-  <si>
-    <t>SecurityBar8K2Timer</t>
-  </si>
-  <si>
-    <t>SecurityBar8K2STATE</t>
-  </si>
-  <si>
-    <t>fimdecurso</t>
-  </si>
-  <si>
-    <t>security</t>
-  </si>
-  <si>
     <t>inputs.h</t>
   </si>
   <si>
-    <t>maq. Estado</t>
-  </si>
-  <si>
-    <t>tempMEM</t>
-  </si>
-  <si>
-    <t>old</t>
-  </si>
-  <si>
-    <t>current</t>
-  </si>
-  <si>
-    <t>timer</t>
-  </si>
-  <si>
-    <t>processed</t>
-  </si>
-  <si>
-    <t>currentType</t>
-  </si>
-  <si>
-    <t>currentKey</t>
-  </si>
-  <si>
-    <t>currentRolling</t>
-  </si>
-  <si>
-    <t>currentSerial</t>
-  </si>
-  <si>
-    <t>currentPosMem</t>
-  </si>
-  <si>
-    <t>button_struct</t>
-  </si>
-  <si>
-    <t>rfCMD</t>
-  </si>
-  <si>
     <t>3A</t>
   </si>
   <si>
-    <t>3B</t>
-  </si>
-  <si>
-    <t>3C</t>
-  </si>
-  <si>
-    <t>3D</t>
-  </si>
-  <si>
-    <t>3E</t>
-  </si>
-  <si>
-    <t>49-4A</t>
-  </si>
-  <si>
-    <t>4B</t>
-  </si>
-  <si>
-    <t>4C</t>
-  </si>
-  <si>
     <t>function number</t>
   </si>
   <si>
     <t>Command List</t>
   </si>
   <si>
-    <t>Abertura_pedonal</t>
-  </si>
-  <si>
-    <t>ctr gate</t>
-  </si>
-  <si>
-    <t>4D</t>
-  </si>
-  <si>
-    <t>StateMotor</t>
-  </si>
-  <si>
     <t>photoCellIsObstructed</t>
   </si>
   <si>
@@ -589,212 +430,32 @@
     <t>FimCurso_OpenIsEnabled</t>
   </si>
   <si>
-    <t>decelerationOpenCurrent</t>
-  </si>
-  <si>
-    <t>decelerationCloseCurrent</t>
-  </si>
-  <si>
-    <t>StartFromButton</t>
-  </si>
-  <si>
-    <t>WaitTimeCloseInitial</t>
-  </si>
-  <si>
-    <t>LastState</t>
-  </si>
-  <si>
-    <t>TriacON</t>
-  </si>
-  <si>
-    <t>InStoping</t>
-  </si>
-  <si>
-    <t>velocityFactor</t>
-  </si>
-  <si>
-    <t>velocityFactorstop</t>
-  </si>
-  <si>
-    <t>AutoInversionActiveStop</t>
-  </si>
-  <si>
-    <t>SoftStopDecrementControl</t>
-  </si>
-  <si>
-    <t>SoftStartDecrementControl</t>
-  </si>
-  <si>
-    <t>Torquerelanty</t>
-  </si>
-  <si>
-    <t>Activatecounter</t>
-  </si>
-  <si>
-    <t>Counter_Learning</t>
-  </si>
-  <si>
-    <t>TimeMaxMotorIsON</t>
-  </si>
-  <si>
     <t>Statedoorcontrol</t>
   </si>
   <si>
-    <t>preflashingcontrol</t>
-  </si>
-  <si>
     <t>PositionActual</t>
   </si>
   <si>
-    <t>DigitSinalizedTemp</t>
-  </si>
-  <si>
-    <t>AutoCloseActive</t>
-  </si>
-  <si>
-    <t>upFaseRGB</t>
-  </si>
-  <si>
-    <t>upFaseFlashligth</t>
-  </si>
-  <si>
-    <t>LearningIsEnabled</t>
-  </si>
-  <si>
-    <t>AutoInversionActive</t>
-  </si>
-  <si>
-    <t>ControlReleCapacitorOpen</t>
-  </si>
-  <si>
-    <t>ControlReleCapacitorClose</t>
-  </si>
-  <si>
-    <t>programinAutomatic</t>
-  </si>
-  <si>
-    <t>photoCellMakeErrorOpen</t>
-  </si>
-  <si>
-    <t>photoCellMakeErrorClose</t>
-  </si>
-  <si>
-    <t>SecurityBarMakeError</t>
-  </si>
-  <si>
-    <t>ActualCurrent</t>
-  </si>
-  <si>
-    <t>ActualHistCurrent</t>
-  </si>
-  <si>
-    <t>ActualComparatorCurrent</t>
-  </si>
-  <si>
-    <t>velocityActual</t>
-  </si>
-  <si>
-    <t>StateFollowIsOn</t>
-  </si>
-  <si>
-    <t>ProgrammingDistanceIs</t>
-  </si>
-  <si>
-    <t>actualCounterMoves</t>
-  </si>
-  <si>
-    <t>DistanceProgrammingActive</t>
-  </si>
-  <si>
-    <t>CurrentAlarmIsOn</t>
-  </si>
-  <si>
-    <t>WorkTimeMaxAlarmState</t>
-  </si>
-  <si>
-    <t>NumberOffErrors</t>
-  </si>
-  <si>
-    <t>InvertionCurrentClosing</t>
-  </si>
-  <si>
-    <t>InvertionCurrentOpening</t>
-  </si>
-  <si>
-    <t>InvertionClosingFromOpen</t>
-  </si>
-  <si>
-    <t>LearningDecelaration</t>
-  </si>
-  <si>
     <t>PositionIsLost</t>
   </si>
   <si>
     <t>StateVersion</t>
   </si>
   <si>
-    <t>Timewalkisactived</t>
-  </si>
-  <si>
-    <t>ADCZeroOffset</t>
-  </si>
-  <si>
-    <t>Control50or60hz</t>
-  </si>
-  <si>
-    <t>frequenciamotor</t>
-  </si>
-  <si>
-    <t>showAP</t>
-  </si>
-  <si>
-    <t>passoAPassoAutoClose</t>
-  </si>
-  <si>
     <t>varSystem</t>
   </si>
   <si>
-    <t>4E</t>
-  </si>
-  <si>
-    <t>4F</t>
-  </si>
-  <si>
-    <t>5A-5B</t>
-  </si>
-  <si>
-    <t>5C</t>
-  </si>
-  <si>
-    <t>5D</t>
-  </si>
-  <si>
-    <t>5E-5F</t>
-  </si>
-  <si>
-    <t>6B</t>
-  </si>
-  <si>
-    <t>6C</t>
-  </si>
-  <si>
-    <t>6F</t>
-  </si>
-  <si>
-    <t>67-68</t>
-  </si>
-  <si>
-    <t>69-6A</t>
-  </si>
-  <si>
-    <t>6D-6E</t>
+    <t>origem</t>
+  </si>
+  <si>
+    <t>38-39</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -837,21 +498,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -942,8 +594,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="47">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -1422,30 +1080,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1474,50 +1108,13 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1638,14 +1235,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1687,62 +1280,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -2065,10 +1622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6891E5-FE77-48FB-B78B-775FB6629AE6}">
-  <dimension ref="B1:J155"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,17 +1641,25 @@
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="57"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="57"/>
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="50"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="32"/>
     </row>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="57"/>
+      <c r="B3" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="59"/>
       <c r="D3" s="28" t="s">
         <v>57</v>
       </c>
@@ -2113,14 +1679,14 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D4" s="29">
         <v>1</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="48">
+      <c r="F4" s="46">
         <v>10</v>
       </c>
       <c r="G4" s="10">
@@ -2133,14 +1699,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="29">
         <v>1</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="47"/>
+      <c r="F5" s="45"/>
       <c r="G5" s="12">
         <v>0</v>
       </c>
@@ -2151,14 +1717,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="29">
         <v>1</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="44">
         <v>11</v>
       </c>
       <c r="G6" s="12">
@@ -2171,14 +1737,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="29">
         <v>1</v>
       </c>
       <c r="E7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="47"/>
+      <c r="F7" s="45"/>
       <c r="G7" s="12">
         <v>0</v>
       </c>
@@ -2189,7 +1755,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="29">
         <v>1</v>
       </c>
@@ -2209,14 +1775,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="29">
         <v>1</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="44">
         <v>13</v>
       </c>
       <c r="G9" s="12">
@@ -2229,14 +1795,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="29">
         <v>1</v>
       </c>
       <c r="E10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="47"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="12">
         <v>0</v>
       </c>
@@ -2247,14 +1813,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="29">
         <v>1</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="44">
         <v>14</v>
       </c>
       <c r="G11" s="12">
@@ -2267,14 +1833,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="29">
         <v>1</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="47"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="12">
         <v>0</v>
       </c>
@@ -2285,14 +1851,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="29">
         <v>1</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="44">
         <v>15</v>
       </c>
       <c r="G13" s="12">
@@ -2305,14 +1871,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="29">
         <v>1</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="47"/>
+      <c r="F14" s="45"/>
       <c r="G14" s="12">
         <v>0</v>
       </c>
@@ -2323,7 +1889,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="29">
         <v>1</v>
       </c>
@@ -2343,7 +1909,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="29">
         <v>1</v>
       </c>
@@ -2470,7 +2036,7 @@
       <c r="E22" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="44" t="s">
         <v>44</v>
       </c>
       <c r="G22" s="12">
@@ -2490,7 +2056,7 @@
       <c r="E23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="47"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="12">
         <v>0</v>
       </c>
@@ -2668,7 +2234,7 @@
       <c r="E32" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="48">
+      <c r="F32" s="46">
         <v>26</v>
       </c>
       <c r="G32" s="13">
@@ -2688,7 +2254,7 @@
       <c r="E33" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="47"/>
+      <c r="F33" s="45"/>
       <c r="G33" s="12">
         <v>0</v>
       </c>
@@ -2701,7 +2267,7 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D34" s="29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>30</v>
@@ -2741,7 +2307,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D36" s="29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E36" s="25" t="s">
         <v>32</v>
@@ -2761,7 +2327,7 @@
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D37" s="31">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E37" s="26" t="s">
         <v>33</v>
@@ -2781,7 +2347,7 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D38" s="29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E38" s="22" t="s">
         <v>34</v>
@@ -2801,7 +2367,7 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D39" s="29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E39" s="24" t="s">
         <v>35</v>
@@ -2821,7 +2387,7 @@
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D40" s="29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>36</v>
@@ -2841,7 +2407,7 @@
     </row>
     <row r="41" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="30">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E41" s="27" t="s">
         <v>37</v>
@@ -2860,47 +2426,33 @@
       </c>
     </row>
     <row r="43" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="73" t="s">
-        <v>153</v>
-      </c>
-      <c r="C43" s="74"/>
+      <c r="B43" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="43"/>
       <c r="D43" s="29">
         <v>1</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E43" s="60" t="s">
         <v>122</v>
       </c>
       <c r="F43" s="16">
         <v>34</v>
       </c>
       <c r="G43" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="75"/>
-      <c r="C44" s="76"/>
-      <c r="D44" s="29">
-        <v>1</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="F44" s="16">
-        <v>34</v>
-      </c>
-      <c r="G44" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="75"/>
-      <c r="C45" s="76"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="61" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="62"/>
       <c r="D45" s="29">
         <v>1</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F45" s="16">
         <v>35</v>
@@ -2910,13 +2462,13 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="77"/>
-      <c r="C46" s="78"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="64"/>
       <c r="D46" s="29">
         <v>1</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F46" s="16">
         <v>35</v>
@@ -2926,1610 +2478,106 @@
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="59"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="45"/>
-    </row>
-    <row r="48" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="60" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="61"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="29">
+        <v>1</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="F47" s="16">
+        <v>36</v>
+      </c>
+      <c r="G47" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="63"/>
+      <c r="C48" s="64"/>
       <c r="D48" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F48" s="16">
         <v>36</v>
       </c>
-      <c r="G48" s="12" t="s">
-        <v>49</v>
+      <c r="G48" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="60"/>
-      <c r="C49" s="61"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="64"/>
       <c r="D49" s="29">
         <v>1</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F49" s="16">
         <v>37</v>
       </c>
       <c r="G49" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="60"/>
-      <c r="C50" s="61"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="64"/>
       <c r="D50" s="29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="F50" s="16">
-        <v>37</v>
-      </c>
-      <c r="G50" s="12">
-        <v>0</v>
+        <v>132</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="60"/>
-      <c r="C51" s="61"/>
+      <c r="B51" s="63"/>
+      <c r="C51" s="64"/>
       <c r="D51" s="29">
         <v>1</v>
       </c>
       <c r="E51" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="F51" s="16">
-        <v>38</v>
+        <v>133</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="G51" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="60"/>
-      <c r="C52" s="61"/>
+      <c r="B52" s="63"/>
+      <c r="C52" s="64"/>
       <c r="D52" s="29">
         <v>1</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="F52" s="16">
-        <v>38</v>
+        <v>134</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="G52" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="60"/>
-      <c r="C53" s="61"/>
-      <c r="D53" s="29">
-        <v>1</v>
-      </c>
-      <c r="E53" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="F53" s="16">
-        <v>39</v>
-      </c>
-      <c r="G53" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="60"/>
-      <c r="C54" s="61"/>
-      <c r="D54" s="29">
-        <v>1</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F54" s="16">
-        <v>39</v>
-      </c>
-      <c r="G54" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="60"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="60"/>
-      <c r="C56" s="63" t="s">
-        <v>150</v>
-      </c>
-      <c r="D56" s="29">
-        <v>1</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="G56" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="60"/>
-      <c r="C57" s="63"/>
-      <c r="D57" s="29">
-        <v>1</v>
-      </c>
-      <c r="E57" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="F57" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="G57" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="60"/>
-      <c r="C58" s="63"/>
-      <c r="D58" s="29">
-        <v>1</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F58" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="G58" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="60"/>
-      <c r="C59" s="63"/>
-      <c r="D59" s="29">
-        <v>1</v>
-      </c>
-      <c r="E59" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="F59" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="G59" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="60"/>
-      <c r="C60" s="63"/>
-      <c r="D60" s="29">
-        <v>1</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="G60" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="60"/>
-      <c r="C61" s="63"/>
-      <c r="D61" s="29">
-        <v>1</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="F61" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="G61" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="60"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="60"/>
-      <c r="C63" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" s="29">
-        <v>1</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="F63" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="G63" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="60"/>
-      <c r="C64" s="63"/>
-      <c r="D64" s="29">
-        <v>1</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="G64" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="60"/>
-      <c r="C65" s="63"/>
-      <c r="D65" s="29">
-        <v>1</v>
-      </c>
-      <c r="E65" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="F65" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="G65" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="60"/>
-      <c r="C66" s="63"/>
-      <c r="D66" s="29">
-        <v>1</v>
-      </c>
-      <c r="E66" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F66" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="G66" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B67" s="60"/>
-      <c r="C67" s="63"/>
-      <c r="D67" s="29">
-        <v>1</v>
-      </c>
-      <c r="E67" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="F67" s="16">
-        <v>40</v>
-      </c>
-      <c r="G67" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B68" s="60"/>
-      <c r="C68" s="63"/>
-      <c r="D68" s="29">
-        <v>1</v>
-      </c>
-      <c r="E68" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="F68" s="16">
-        <v>40</v>
-      </c>
-      <c r="G68" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="60"/>
-      <c r="C69" s="63"/>
-      <c r="D69" s="29">
-        <v>1</v>
-      </c>
-      <c r="E69" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="F69" s="16">
-        <v>41</v>
-      </c>
-      <c r="G69" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="60"/>
-      <c r="C70" s="63"/>
-      <c r="D70" s="29">
-        <v>1</v>
-      </c>
-      <c r="E70" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="F70" s="16">
-        <v>41</v>
-      </c>
-      <c r="G70" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="60"/>
-      <c r="C71" s="63"/>
-      <c r="D71" s="29">
-        <v>1</v>
-      </c>
-      <c r="E71" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="F71" s="16">
-        <v>42</v>
-      </c>
-      <c r="G71" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="60"/>
-      <c r="C72" s="63"/>
-      <c r="D72" s="29">
-        <v>1</v>
-      </c>
-      <c r="E72" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="F72" s="16">
-        <v>42</v>
-      </c>
-      <c r="G72" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="60"/>
-      <c r="C73" s="63"/>
-      <c r="D73" s="29">
-        <v>1</v>
-      </c>
-      <c r="E73" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="F73" s="16">
-        <v>43</v>
-      </c>
-      <c r="G73" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="60"/>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="60"/>
-      <c r="C75" s="62"/>
-      <c r="D75" s="29">
-        <v>1</v>
-      </c>
-      <c r="E75" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="F75" s="16">
-        <v>44</v>
-      </c>
-      <c r="G75" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="60"/>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="60"/>
-      <c r="C77" s="64" t="s">
-        <v>164</v>
-      </c>
-      <c r="D77" s="29">
-        <v>1</v>
-      </c>
-      <c r="E77" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="F77" s="16">
-        <v>45</v>
-      </c>
-      <c r="G77" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="60"/>
-      <c r="C78" s="64"/>
-      <c r="D78" s="29">
-        <v>1</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="F78" s="16">
-        <v>45</v>
-      </c>
-      <c r="G78" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="60"/>
-      <c r="C79" s="64"/>
-      <c r="D79" s="29">
-        <v>1</v>
-      </c>
-      <c r="E79" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="F79" s="16">
-        <v>46</v>
-      </c>
-      <c r="G79" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="60"/>
-      <c r="C80" s="64"/>
-      <c r="D80" s="29">
-        <v>1</v>
-      </c>
-      <c r="E80" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="F80" s="16">
-        <v>46</v>
-      </c>
-      <c r="G80" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="60"/>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="60"/>
-      <c r="C82" s="60" t="s">
-        <v>165</v>
-      </c>
-      <c r="D82" s="29">
-        <v>1</v>
-      </c>
-      <c r="E82" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="F82" s="16">
-        <v>47</v>
-      </c>
-      <c r="G82" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" s="60"/>
-      <c r="C83" s="60"/>
-      <c r="D83" s="29">
-        <v>1</v>
-      </c>
-      <c r="E83" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="F83" s="16">
-        <v>47</v>
-      </c>
-      <c r="G83" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B84" s="60"/>
-      <c r="C84" s="60"/>
-      <c r="D84" s="29">
-        <v>2</v>
-      </c>
-      <c r="E84" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="F84" s="16">
-        <v>48</v>
-      </c>
-      <c r="G84" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="60"/>
-      <c r="C85" s="60"/>
-      <c r="D85" s="29">
-        <v>4</v>
-      </c>
-      <c r="E85" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="F85" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="G85" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="60"/>
-      <c r="C86" s="60"/>
-      <c r="D86" s="29">
-        <v>1</v>
-      </c>
-      <c r="E86" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="F86" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G86" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="60"/>
-      <c r="C87" s="60"/>
-      <c r="D87" s="29">
-        <v>1</v>
-      </c>
-      <c r="E87" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="F87" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G87" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="60"/>
-      <c r="C88" s="60"/>
-      <c r="D88" s="29">
-        <v>1</v>
-      </c>
-      <c r="E88" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="F88" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="G88" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="65" t="s">
-        <v>177</v>
-      </c>
-      <c r="C90" s="66"/>
-      <c r="D90" s="29">
-        <v>1</v>
-      </c>
-      <c r="E90" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="F90" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="G90" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="70" t="s">
-        <v>238</v>
-      </c>
-      <c r="C92" s="67"/>
-      <c r="D92" s="29">
-        <v>1</v>
-      </c>
-      <c r="E92" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="F92" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="G92" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="71"/>
-      <c r="C93" s="68"/>
-      <c r="D93" s="29">
-        <v>1</v>
-      </c>
-      <c r="E93" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="F93" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="G93" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="71"/>
-      <c r="C94" s="68"/>
-      <c r="D94" s="29">
-        <v>1</v>
-      </c>
-      <c r="E94" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="F94" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="G94" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="71"/>
-      <c r="C95" s="68"/>
-      <c r="D95" s="29">
-        <v>1</v>
-      </c>
-      <c r="E95" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="F95" s="16">
-        <v>50</v>
-      </c>
-      <c r="G95" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="71"/>
-      <c r="C96" s="68"/>
-      <c r="D96" s="29">
-        <v>1</v>
-      </c>
-      <c r="E96" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="F96" s="16">
-        <v>50</v>
-      </c>
-      <c r="G96" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="71"/>
-      <c r="C97" s="68"/>
-      <c r="D97" s="29">
-        <v>2</v>
-      </c>
-      <c r="E97" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="F97" s="16">
-        <v>51</v>
-      </c>
-      <c r="G97" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="71"/>
-      <c r="C98" s="68"/>
-      <c r="D98" s="29">
-        <v>2</v>
-      </c>
-      <c r="E98" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="F98" s="16">
-        <v>52</v>
-      </c>
-      <c r="G98" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="71"/>
-      <c r="C99" s="68"/>
-      <c r="D99" s="29">
-        <v>1</v>
-      </c>
-      <c r="E99" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="F99" s="16">
-        <v>53</v>
-      </c>
-      <c r="G99" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="71"/>
-      <c r="C100" s="68"/>
-      <c r="D100" s="29">
-        <v>1</v>
-      </c>
-      <c r="E100" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="F100" s="16">
-        <v>53</v>
-      </c>
-      <c r="G100" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="71"/>
-      <c r="C101" s="68"/>
-      <c r="D101" s="29">
-        <v>1</v>
-      </c>
-      <c r="E101" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="F101" s="16">
-        <v>54</v>
-      </c>
-      <c r="G101" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B102" s="71"/>
-      <c r="C102" s="68"/>
-      <c r="D102" s="29">
-        <v>1</v>
-      </c>
-      <c r="E102" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="F102" s="16">
-        <v>54</v>
-      </c>
-      <c r="G102" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="71"/>
-      <c r="C103" s="68"/>
-      <c r="D103" s="29">
-        <v>1</v>
-      </c>
-      <c r="E103" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="F103" s="16">
-        <v>55</v>
-      </c>
-      <c r="G103" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="71"/>
-      <c r="C104" s="68"/>
-      <c r="D104" s="29">
-        <v>1</v>
-      </c>
-      <c r="E104" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="F104" s="16">
-        <v>55</v>
-      </c>
-      <c r="G104" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="71"/>
-      <c r="C105" s="68"/>
-      <c r="D105" s="29">
-        <v>2</v>
-      </c>
-      <c r="E105" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="F105" s="16">
-        <v>56</v>
-      </c>
-      <c r="G105" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="71"/>
-      <c r="C106" s="68"/>
-      <c r="D106" s="29">
-        <v>2</v>
-      </c>
-      <c r="E106" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="F106" s="16">
-        <v>57</v>
-      </c>
-      <c r="G106" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="71"/>
-      <c r="C107" s="68"/>
-      <c r="D107" s="29">
-        <v>1</v>
-      </c>
-      <c r="E107" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="F107" s="16">
-        <v>58</v>
-      </c>
-      <c r="G107" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="71"/>
-      <c r="C108" s="68"/>
-      <c r="D108" s="29">
-        <v>1</v>
-      </c>
-      <c r="E108" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="F108" s="16">
-        <v>58</v>
-      </c>
-      <c r="G108" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="71"/>
-      <c r="C109" s="68"/>
-      <c r="D109" s="29">
-        <v>1</v>
-      </c>
-      <c r="E109" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="F109" s="16">
-        <v>59</v>
-      </c>
-      <c r="G109" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="71"/>
-      <c r="C110" s="68"/>
-      <c r="D110" s="29">
-        <v>1</v>
-      </c>
-      <c r="E110" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="F110" s="16">
-        <v>59</v>
-      </c>
-      <c r="G110" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="71"/>
-      <c r="C111" s="68"/>
-      <c r="D111" s="29">
-        <v>4</v>
-      </c>
-      <c r="E111" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="F111" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="G111" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="71"/>
-      <c r="C112" s="68"/>
-      <c r="D112" s="29">
-        <v>1</v>
-      </c>
-      <c r="E112" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="F112" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="G112" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="71"/>
-      <c r="C113" s="68"/>
-      <c r="D113" s="29">
-        <v>1</v>
-      </c>
-      <c r="E113" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="F113" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="G113" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B114" s="71"/>
-      <c r="C114" s="69"/>
-      <c r="D114" s="29">
-        <v>1</v>
-      </c>
-      <c r="E114" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="F114" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="G114" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B115" s="71"/>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="71"/>
-      <c r="C116" s="67"/>
-      <c r="D116" s="29">
-        <v>4</v>
-      </c>
-      <c r="E116" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="F116" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="G116" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B117" s="71"/>
-      <c r="C117" s="68"/>
-      <c r="D117" s="29">
-        <v>1</v>
-      </c>
-      <c r="E117" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="F117" s="16">
-        <v>60</v>
-      </c>
-      <c r="G117" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B118" s="71"/>
-      <c r="C118" s="68"/>
-      <c r="D118" s="29">
-        <v>1</v>
-      </c>
-      <c r="E118" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="F118" s="16">
-        <v>60</v>
-      </c>
-      <c r="G118" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119" s="71"/>
-      <c r="C119" s="68"/>
-      <c r="D119" s="29">
-        <v>1</v>
-      </c>
-      <c r="E119" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="F119" s="16">
-        <v>61</v>
-      </c>
-      <c r="G119" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B120" s="71"/>
-      <c r="C120" s="68"/>
-      <c r="D120" s="29">
-        <v>1</v>
-      </c>
-      <c r="E120" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="F120" s="16">
-        <v>61</v>
-      </c>
-      <c r="G120" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B121" s="71"/>
-      <c r="C121" s="68"/>
-      <c r="D121" s="29">
-        <v>1</v>
-      </c>
-      <c r="E121" s="24" t="s">
-        <v>207</v>
-      </c>
-      <c r="F121" s="16">
-        <v>62</v>
-      </c>
-      <c r="G121" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B122" s="71"/>
-      <c r="C122" s="69"/>
-      <c r="D122" s="29">
-        <v>1</v>
-      </c>
-      <c r="E122" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="F122" s="16">
-        <v>62</v>
-      </c>
-      <c r="G122" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B123" s="71"/>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B124" s="71"/>
-      <c r="C124" s="67"/>
-      <c r="D124" s="29">
-        <v>1</v>
-      </c>
-      <c r="E124" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="F124" s="16">
-        <v>63</v>
-      </c>
-      <c r="G124" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="71"/>
-      <c r="C125" s="68"/>
-      <c r="D125" s="29">
-        <v>1</v>
-      </c>
-      <c r="E125" s="24" t="s">
-        <v>210</v>
-      </c>
-      <c r="F125" s="16">
-        <v>63</v>
-      </c>
-      <c r="G125" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B126" s="71"/>
-      <c r="C126" s="69"/>
-      <c r="D126" s="29">
-        <v>1</v>
-      </c>
-      <c r="E126" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="F126" s="16">
-        <v>64</v>
-      </c>
-      <c r="G126" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="71"/>
-    </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B128" s="71"/>
-      <c r="C128" s="67"/>
-      <c r="D128" s="29">
-        <v>1</v>
-      </c>
-      <c r="E128" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="F128" s="16">
-        <v>65</v>
-      </c>
-      <c r="G128" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B129" s="71"/>
-      <c r="C129" s="68"/>
-      <c r="D129" s="29">
-        <v>1</v>
-      </c>
-      <c r="E129" s="24" t="s">
-        <v>213</v>
-      </c>
-      <c r="F129" s="16">
-        <v>65</v>
-      </c>
-      <c r="G129" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B130" s="71"/>
-      <c r="C130" s="68"/>
-      <c r="D130" s="29">
-        <v>2</v>
-      </c>
-      <c r="E130" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="F130" s="16">
-        <v>66</v>
-      </c>
-      <c r="G130" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B131" s="71"/>
-      <c r="C131" s="68"/>
-      <c r="D131" s="29">
-        <v>4</v>
-      </c>
-      <c r="E131" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="F131" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="G131" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B132" s="71"/>
-      <c r="C132" s="68"/>
-      <c r="D132" s="29">
-        <v>4</v>
-      </c>
-      <c r="E132" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="F132" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="G132" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B133" s="71"/>
-      <c r="C133" s="68"/>
-      <c r="D133" s="29">
-        <v>2</v>
-      </c>
-      <c r="E133" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="F133" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="G133" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="71"/>
-      <c r="C134" s="68"/>
-      <c r="D134" s="29">
-        <v>1</v>
-      </c>
-      <c r="E134" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="F134" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="G134" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B135" s="71"/>
-      <c r="C135" s="68"/>
-      <c r="D135" s="29">
-        <v>1</v>
-      </c>
-      <c r="E135" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="F135" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="G135" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B136" s="71"/>
-      <c r="C136" s="68"/>
-      <c r="D136" s="29">
-        <v>4</v>
-      </c>
-      <c r="E136" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="F136" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="G136" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B137" s="71"/>
-      <c r="C137" s="68"/>
-      <c r="D137" s="29">
-        <v>1</v>
-      </c>
-      <c r="E137" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="F137" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="G137" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B138" s="71"/>
-      <c r="C138" s="68"/>
-      <c r="D138" s="29">
-        <v>1</v>
-      </c>
-      <c r="E138" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="F138" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="G138" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B139" s="71"/>
-      <c r="C139" s="68"/>
-      <c r="D139" s="29">
-        <v>1</v>
-      </c>
-      <c r="E139" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="F139" s="16">
-        <v>70</v>
-      </c>
-      <c r="G139" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B140" s="71"/>
-      <c r="C140" s="68"/>
-      <c r="D140" s="29">
-        <v>1</v>
-      </c>
-      <c r="E140" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="F140" s="16">
-        <v>70</v>
-      </c>
-      <c r="G140" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B141" s="71"/>
-      <c r="C141" s="68"/>
-      <c r="D141" s="29">
-        <v>1</v>
-      </c>
-      <c r="E141" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="F141" s="16">
-        <v>71</v>
-      </c>
-      <c r="G141" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B142" s="71"/>
-      <c r="C142" s="68"/>
-      <c r="D142" s="29">
-        <v>1</v>
-      </c>
-      <c r="E142" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="F142" s="16">
-        <v>71</v>
-      </c>
-      <c r="G142" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="71"/>
-      <c r="C143" s="68"/>
-      <c r="D143" s="29">
-        <v>1</v>
-      </c>
-      <c r="E143" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="F143" s="16">
-        <v>72</v>
-      </c>
-      <c r="G143" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B144" s="71"/>
-      <c r="C144" s="68"/>
-      <c r="D144" s="29">
-        <v>1</v>
-      </c>
-      <c r="E144" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="F144" s="16">
-        <v>72</v>
-      </c>
-      <c r="G144" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B145" s="71"/>
-      <c r="C145" s="68"/>
-      <c r="D145" s="29">
-        <v>1</v>
-      </c>
-      <c r="E145" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="F145" s="16">
-        <v>73</v>
-      </c>
-      <c r="G145" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B146" s="71"/>
-      <c r="C146" s="68"/>
-      <c r="D146" s="29">
-        <v>1</v>
-      </c>
-      <c r="E146" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="F146" s="16">
-        <v>73</v>
-      </c>
-      <c r="G146" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B147" s="71"/>
-      <c r="C147" s="68"/>
-      <c r="D147" s="29">
-        <v>1</v>
-      </c>
-      <c r="E147" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="F147" s="16">
-        <v>74</v>
-      </c>
-      <c r="G147" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B148" s="71"/>
-      <c r="C148" s="69"/>
-      <c r="D148" s="29">
-        <v>1</v>
-      </c>
-      <c r="E148" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="F148" s="16">
-        <v>74</v>
-      </c>
-      <c r="G148" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B149" s="71"/>
-    </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B150" s="71"/>
-      <c r="C150" s="67"/>
-      <c r="D150" s="29">
-        <v>2</v>
-      </c>
-      <c r="E150" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="F150" s="16">
-        <v>75</v>
-      </c>
-      <c r="G150" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B151" s="71"/>
-      <c r="C151" s="68"/>
-      <c r="D151" s="29">
-        <v>1</v>
-      </c>
-      <c r="E151" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="F151" s="16">
-        <v>76</v>
-      </c>
-      <c r="G151" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B152" s="71"/>
-      <c r="C152" s="69"/>
-      <c r="D152" s="29">
-        <v>1</v>
-      </c>
-      <c r="E152" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="F152" s="16">
-        <v>76</v>
-      </c>
-      <c r="G152" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B153" s="71"/>
-    </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B154" s="71"/>
-      <c r="C154" s="67"/>
-      <c r="D154" s="29">
-        <v>1</v>
-      </c>
-      <c r="E154" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="F154" s="16">
-        <v>77</v>
-      </c>
-      <c r="G154" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B155" s="72"/>
-      <c r="C155" s="69"/>
-      <c r="D155" s="29">
-        <v>1</v>
-      </c>
-      <c r="E155" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="F155" s="16">
-        <v>77</v>
-      </c>
-      <c r="G155" s="12">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="C77:C80"/>
-    <mergeCell ref="C82:C88"/>
-    <mergeCell ref="B48:B88"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B92:B155"/>
-    <mergeCell ref="C92:C114"/>
-    <mergeCell ref="C116:C122"/>
-    <mergeCell ref="C124:C126"/>
-    <mergeCell ref="C128:C148"/>
-    <mergeCell ref="C150:C152"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="C56:C61"/>
-    <mergeCell ref="C63:C73"/>
-    <mergeCell ref="C48:C54"/>
-    <mergeCell ref="B43:C46"/>
+  <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B45:C52"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="H2:I2"/>
@@ -4549,16 +2597,16 @@
   <dimension ref="B1:AA25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
@@ -4581,17 +2629,17 @@
     </row>
     <row r="2" spans="2:27" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B2" s="33"/>
-      <c r="C2" s="51" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
+      <c r="C2" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
       <c r="L2" s="33"/>
       <c r="M2" s="33"/>
       <c r="N2" s="33"/>
@@ -4611,23 +2659,23 @@
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="33"/>
-      <c r="C3" s="56" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" s="57" t="s">
+      <c r="C3" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="52" t="s">
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="50" t="s">
         <v>110</v>
       </c>
       <c r="L3" s="33"/>
@@ -4649,9 +2697,9 @@
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="33"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="58"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="34" t="s">
         <v>69</v>
       </c>
@@ -4667,7 +2715,7 @@
       <c r="J4" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="52"/>
+      <c r="K4" s="50"/>
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
       <c r="N4" s="33"/>
@@ -4855,7 +2903,7 @@
       <c r="L8" s="33"/>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="51" t="s">
         <v>120</v>
       </c>
       <c r="C9" s="41">
@@ -4888,7 +2936,7 @@
       <c r="L9" s="33"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="53"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="41">
         <v>5</v>
       </c>
@@ -4919,7 +2967,7 @@
       <c r="L10" s="33"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="53"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="41">
         <v>6</v>
       </c>
@@ -4950,7 +2998,7 @@
       <c r="L11" s="33"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="53"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="41">
         <v>7</v>
       </c>
@@ -4981,7 +3029,7 @@
       <c r="L12" s="33"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="53"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="41">
         <v>8</v>
       </c>
@@ -5012,7 +3060,7 @@
       <c r="L13" s="33"/>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B14" s="53"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="41">
         <v>9</v>
       </c>
@@ -5043,7 +3091,7 @@
       <c r="L14" s="33"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B15" s="53"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="41">
         <v>10</v>
       </c>
@@ -5074,7 +3122,7 @@
       <c r="L15" s="33"/>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="52" t="s">
         <v>121</v>
       </c>
       <c r="C16" s="41">
@@ -5102,12 +3150,12 @@
         <v>74</v>
       </c>
       <c r="K16" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="33"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="41">
         <v>12</v>
       </c>
@@ -5133,12 +3181,12 @@
         <v>74</v>
       </c>
       <c r="K17" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="33"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="54"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="41">
         <v>13</v>
       </c>
@@ -5164,12 +3212,12 @@
         <v>74</v>
       </c>
       <c r="K18" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="33"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="54"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="41">
         <v>14</v>
       </c>
@@ -5195,12 +3243,12 @@
         <v>74</v>
       </c>
       <c r="K19" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="33"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="54"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="41">
         <v>15</v>
       </c>
@@ -5226,12 +3274,12 @@
         <v>74</v>
       </c>
       <c r="K20" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="33"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="54"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="41">
         <v>16</v>
       </c>
@@ -5257,12 +3305,12 @@
         <v>74</v>
       </c>
       <c r="K21" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="33"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="54"/>
+      <c r="B22" s="52"/>
       <c r="C22" s="41">
         <v>17</v>
       </c>
@@ -5288,7 +3336,7 @@
         <v>74</v>
       </c>
       <c r="K22" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="33"/>
     </row>

</xml_diff>